<commit_message>
Updated recording and attendance for Yufeng Lai
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CB2D93-CA39-4105-891A-1A5024460448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BFEE53-398A-4530-8454-07C0043CFE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="MS Symposium" sheetId="3" r:id="rId1"/>
@@ -1106,46 +1106,46 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5013,7 +5013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A92331-1E38-48FD-9605-0D81D4E71360}">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -5100,7 +5100,7 @@
       </c>
       <c r="Q4">
         <f>'2024 - Fall'!K3</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -5124,7 +5124,7 @@
       </c>
       <c r="Q5">
         <f>'2024 - Fall'!K4</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="Q6">
         <f>'2024 - Fall'!K5</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -5166,7 +5166,7 @@
       </c>
       <c r="Q7">
         <f>'2024 - Fall'!K6</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -5190,7 +5190,7 @@
       </c>
       <c r="Q8">
         <f>'2024 - Fall'!K7</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="Q9">
         <f>'2024 - Fall'!K8</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="Q10">
         <f>'2024 - Fall'!K9</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -5255,7 +5255,7 @@
       </c>
       <c r="Q11">
         <f>'2024 - Fall'!K10</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -5272,7 +5272,7 @@
       </c>
       <c r="Q12">
         <f>'2024 - Fall'!K11</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5323,7 +5323,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.3">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
@@ -5572,8 +5572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5686,16 +5686,22 @@
       <c r="F3" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="G3" s="1">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1">
+        <v>4</v>
+      </c>
       <c r="I3" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K16" si="1">K2+I3</f>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>233</v>
@@ -5729,7 +5735,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>234</v>
@@ -5763,7 +5769,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>233</v>
@@ -5794,7 +5800,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>234</v>
@@ -5828,7 +5834,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>233</v>
@@ -5859,7 +5865,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>234</v>
@@ -5893,7 +5899,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>234</v>
@@ -5924,7 +5930,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>233</v>
@@ -5955,7 +5961,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>234</v>
@@ -5986,7 +5992,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>234</v>
@@ -6020,7 +6026,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>233</v>
@@ -6054,7 +6060,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>233</v>
@@ -6088,7 +6094,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>234</v>
@@ -6119,7 +6125,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>234</v>
@@ -6136,15 +6142,15 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6159,15 +6165,15 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6186,7 +6192,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.21052631578947367</v>
+        <v>0.25</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated the attendance from last week
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D48125-D1B5-44D1-8207-615C51CBD675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3AA777-D502-4790-83F9-87863D4FC1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -1109,43 +1109,43 @@
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>54</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="Q5">
         <f>'2024 - Fall'!K4</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="Q6">
         <f>'2024 - Fall'!K5</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -5166,7 +5166,7 @@
       </c>
       <c r="Q7">
         <f>'2024 - Fall'!K6</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -5190,7 +5190,7 @@
       </c>
       <c r="Q8">
         <f>'2024 - Fall'!K7</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="Q9">
         <f>'2024 - Fall'!K8</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="Q10">
         <f>'2024 - Fall'!K9</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -5255,7 +5255,7 @@
       </c>
       <c r="Q11">
         <f>'2024 - Fall'!K10</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -5272,7 +5272,7 @@
       </c>
       <c r="Q12">
         <f>'2024 - Fall'!K11</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5323,7 +5323,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.3">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
@@ -5727,21 +5727,21 @@
         <v>61</v>
       </c>
       <c r="G4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="1">
         <v>9</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
       <c r="K4">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>234</v>
@@ -5775,7 +5775,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>233</v>
@@ -5806,7 +5806,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>234</v>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>233</v>
@@ -5871,7 +5871,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>234</v>
@@ -5905,7 +5905,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>234</v>
@@ -5936,7 +5936,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>233</v>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>234</v>
@@ -5998,7 +5998,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>234</v>
@@ -6032,7 +6032,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>233</v>
@@ -6066,7 +6066,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>233</v>
@@ -6100,7 +6100,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>234</v>
@@ -6131,7 +6131,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>234</v>
@@ -6148,7 +6148,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
@@ -6156,7 +6156,7 @@
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6171,7 +6171,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>13</v>
+        <v>12.666666666666666</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
@@ -6179,7 +6179,7 @@
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>18</v>
+        <v>17.666666666666664</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6198,7 +6198,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.23684210526315788</v>
+        <v>0.23245614035087717</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added slides and recording for Abel Brodeur workshop
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3AA777-D502-4790-83F9-87863D4FC1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D5A853-F916-4F4C-9DDC-4ECFF065FC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="236">
   <si>
     <t>Date</t>
   </si>
@@ -757,6 +757,9 @@
   </si>
   <si>
     <t>Carmen</t>
+  </si>
+  <si>
+    <t>JMC</t>
   </si>
 </sst>
 </file>
@@ -1112,40 +1115,40 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5014,7 +5017,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5148,7 +5151,7 @@
       </c>
       <c r="Q6">
         <f>'2024 - Fall'!K5</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -5166,7 +5169,7 @@
       </c>
       <c r="Q7">
         <f>'2024 - Fall'!K6</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -5190,7 +5193,7 @@
       </c>
       <c r="Q8">
         <f>'2024 - Fall'!K7</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -5214,7 +5217,7 @@
       </c>
       <c r="Q9">
         <f>'2024 - Fall'!K8</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -5238,7 +5241,7 @@
       </c>
       <c r="Q10">
         <f>'2024 - Fall'!K9</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -5255,7 +5258,7 @@
       </c>
       <c r="Q11">
         <f>'2024 - Fall'!K10</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -5272,7 +5275,7 @@
       </c>
       <c r="Q12">
         <f>'2024 - Fall'!K11</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -5289,7 +5292,7 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5306,7 +5309,7 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5323,7 +5326,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5340,7 +5343,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.3">
@@ -5353,7 +5356,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
@@ -5573,7 +5576,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5587,7 +5590,7 @@
     <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="1"/>
   </cols>
@@ -5659,6 +5662,9 @@
         <f t="shared" ref="I2:I16" si="0">SUM(G2:H2)</f>
         <v>16</v>
       </c>
+      <c r="J2" t="s">
+        <v>235</v>
+      </c>
       <c r="K2">
         <f>I2</f>
         <v>16</v>
@@ -5766,16 +5772,22 @@
       <c r="F5" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>226</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>233</v>
@@ -5804,9 +5816,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J6" t="s">
+        <v>235</v>
+      </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>234</v>
@@ -5840,7 +5855,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>233</v>
@@ -5871,7 +5886,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>234</v>
@@ -5905,7 +5920,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>234</v>
@@ -5934,9 +5949,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J10" t="s">
+        <v>235</v>
+      </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>233</v>
@@ -5965,9 +5983,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J11" t="s">
+        <v>235</v>
+      </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>234</v>
@@ -5996,9 +6017,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J12" t="s">
+        <v>235</v>
+      </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>234</v>
@@ -6032,7 +6056,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>233</v>
@@ -6066,7 +6090,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>233</v>
@@ -6100,7 +6124,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>234</v>
@@ -6129,9 +6153,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J16" t="s">
+        <v>235</v>
+      </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>234</v>
@@ -6148,15 +6175,15 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6171,7 +6198,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>12.666666666666666</v>
+        <v>10.75</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
@@ -6179,7 +6206,7 @@
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>17.666666666666664</v>
+        <v>15.75</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6198,7 +6225,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.23245614035087717</v>
+        <v>0.20723684210526316</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>
@@ -6258,9 +6285,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9DA028-C994-415A-B404-123C1AD93D08}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6480,6 +6507,9 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
+      <c r="J6" t="s">
+        <v>235</v>
+      </c>
       <c r="K6">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -6622,6 +6652,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="J10" t="s">
+        <v>235</v>
+      </c>
       <c r="K10">
         <f t="shared" si="1"/>
         <v>132</v>
@@ -6763,6 +6796,9 @@
       <c r="I14" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>235</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
@@ -6947,8 +6983,8 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7029,6 +7065,9 @@
         <f t="shared" ref="I2:I17" si="0">SUM(G2:H2)</f>
         <v>10</v>
       </c>
+      <c r="J2" t="s">
+        <v>235</v>
+      </c>
       <c r="K2">
         <f>I2</f>
         <v>10</v>
@@ -7100,6 +7139,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="J4" t="s">
+        <v>235</v>
+      </c>
       <c r="K4">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -7353,6 +7395,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="J11" t="s">
+        <v>235</v>
+      </c>
       <c r="K11">
         <f t="shared" si="1"/>
         <v>158</v>
@@ -7458,6 +7503,9 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="J14" t="s">
+        <v>235</v>
+      </c>
       <c r="K14">
         <f t="shared" si="1"/>
         <v>204</v>
@@ -7491,6 +7539,9 @@
       <c r="I15" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>235</v>
       </c>
       <c r="K15">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Added Monique as a discussant for Evan's presentation
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D5A853-F916-4F4C-9DDC-4ECFF065FC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C22A2E-AA25-48F3-B51D-D07962E5D032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="236">
   <si>
     <t>Date</t>
   </si>
@@ -5575,8 +5575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5876,6 +5876,9 @@
       </c>
       <c r="E8" s="17" t="s">
         <v>196</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Adding info about Jiuchen seminar attendance
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Phd\Jobs\Apec seminar\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3AA777-D502-4790-83F9-87863D4FC1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C8ED81-CB0E-4137-904F-CCF1AF73B492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="MS Symposium" sheetId="3" r:id="rId1"/>
@@ -1112,40 +1112,40 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>53</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4741,12 +4741,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="8" width="20.77734375" customWidth="1"/>
+    <col min="1" max="8" width="20.76953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>117</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="59" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
@@ -4808,7 +4808,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10"/>
@@ -4817,7 +4817,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10"/>
@@ -4829,7 +4829,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10"/>
@@ -4841,7 +4841,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="10"/>
@@ -4850,7 +4850,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10"/>
@@ -4859,7 +4859,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
@@ -4868,7 +4868,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
@@ -4877,7 +4877,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
@@ -4886,7 +4886,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="10"/>
@@ -4895,7 +4895,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="10"/>
@@ -4904,7 +4904,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="10"/>
@@ -4913,7 +4913,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="10"/>
@@ -4922,7 +4922,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="10"/>
@@ -4931,7 +4931,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:8" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A17:C17"/>
@@ -5017,24 +5017,24 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" customWidth="1"/>
-    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.6640625" customWidth="1"/>
-    <col min="20" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.2265625" customWidth="1"/>
+    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.2265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.6796875" customWidth="1"/>
+    <col min="20" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A1" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A3" s="13" t="s">
         <v>123</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A4" s="13" t="s">
         <v>124</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A5" s="13" t="s">
         <v>126</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A6" s="13" t="s">
         <v>127</v>
       </c>
@@ -5148,10 +5148,10 @@
       </c>
       <c r="Q6">
         <f>'2024 - Fall'!K5</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A7" s="14"/>
       <c r="N7">
         <v>5</v>
@@ -5166,10 +5166,10 @@
       </c>
       <c r="Q7">
         <f>'2024 - Fall'!K6</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
@@ -5190,10 +5190,10 @@
       </c>
       <c r="Q8">
         <f>'2024 - Fall'!K7</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -5214,10 +5214,10 @@
       </c>
       <c r="Q9">
         <f>'2024 - Fall'!K8</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -5238,10 +5238,10 @@
       </c>
       <c r="Q10">
         <f>'2024 - Fall'!K9</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N11">
         <v>9</v>
       </c>
@@ -5255,10 +5255,10 @@
       </c>
       <c r="Q11">
         <f>'2024 - Fall'!K10</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N12">
         <v>10</v>
       </c>
@@ -5272,10 +5272,10 @@
       </c>
       <c r="Q12">
         <f>'2024 - Fall'!K11</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N13">
         <v>11</v>
       </c>
@@ -5289,10 +5289,10 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N14">
         <v>12</v>
       </c>
@@ -5306,10 +5306,10 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N15">
         <v>13</v>
       </c>
@@ -5323,10 +5323,10 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N16">
         <v>14</v>
       </c>
@@ -5340,10 +5340,10 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="14:26" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N17">
         <v>15</v>
       </c>
@@ -5353,20 +5353,20 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="14:26" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N19" s="20" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N21" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N22" t="s">
         <v>146</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N23">
         <f>1+1+1+1+1</f>
         <v>5</v>
@@ -5391,7 +5391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N24" s="16">
         <f>N23/SUM($N$23:$P$23)</f>
         <v>0.38461538461538464</v>
@@ -5405,12 +5405,12 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="26" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N26" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N27" t="s">
         <v>157</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N28">
         <f>1+1+1+1+1+1+1</f>
         <v>7</v>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N29" s="16">
         <f t="shared" ref="N29:Z29" si="0">N28/SUM($N$28:$Z$28)</f>
         <v>0.2413793103448276</v>
@@ -5573,26 +5573,26 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.2265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.31640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.31640625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.86328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>173</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>174</v>
       </c>
@@ -5766,22 +5766,28 @@
       <c r="F5" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1">
+        <v>5</v>
+      </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>226</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="59" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>175</v>
       </c>
@@ -5800,19 +5806,25 @@
       <c r="F6" s="19" t="s">
         <v>93</v>
       </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7</v>
+      </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>176</v>
       </c>
@@ -5840,13 +5852,13 @@
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>177</v>
       </c>
@@ -5871,13 +5883,13 @@
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>178</v>
       </c>
@@ -5905,13 +5917,13 @@
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>179</v>
       </c>
@@ -5936,13 +5948,13 @@
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>180</v>
       </c>
@@ -5967,13 +5979,13 @@
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>181</v>
       </c>
@@ -5998,13 +6010,13 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -6032,13 +6044,13 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>183</v>
       </c>
@@ -6066,13 +6078,13 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>184</v>
       </c>
@@ -6100,13 +6112,13 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>185</v>
       </c>
@@ -6131,13 +6143,13 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -6148,19 +6160,19 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -6171,21 +6183,21 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>12.666666666666666</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>5</v>
+        <v>5.4</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>17.666666666666664</v>
+        <v>15.200000000000001</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -6198,49 +6210,49 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.23245614035087717</v>
+        <v>0.2</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C25" s="17"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C26" s="17"/>
       <c r="D26" s="18"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C27" s="17"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C31" s="17"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C32" s="17"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C33" s="17"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C34" s="17"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C35" s="17"/>
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C36" s="17"/>
       <c r="D36" s="18"/>
     </row>
@@ -6263,21 +6275,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.2265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="8" customWidth="1"/>
-    <col min="4" max="4" width="45.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="4" max="4" width="45.76953125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.6796875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.2265625" customWidth="1"/>
+    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6312,7 +6324,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="59" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -6346,7 +6358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -6380,7 +6392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -6414,7 +6426,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -6451,7 +6463,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -6485,7 +6497,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -6522,7 +6534,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="27.25" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -6556,7 +6568,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
@@ -6593,7 +6605,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -6627,7 +6639,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -6664,7 +6676,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -6701,7 +6713,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -6735,7 +6747,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="27.25" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -6769,7 +6781,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
@@ -6806,7 +6818,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -6840,7 +6852,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -6863,7 +6875,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -6888,7 +6900,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -6907,29 +6919,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E29"/>
     </row>
   </sheetData>
@@ -6951,21 +6963,21 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.2265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.31640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.31640625" customWidth="1"/>
+    <col min="5" max="5" width="15.31640625" customWidth="1"/>
+    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -7000,7 +7012,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="59" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -7034,7 +7046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -7071,7 +7083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -7105,7 +7117,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -7139,7 +7151,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -7176,7 +7188,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -7213,7 +7225,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -7250,7 +7262,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -7287,7 +7299,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -7324,7 +7336,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -7358,7 +7370,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -7395,7 +7407,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -7429,7 +7441,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -7463,7 +7475,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -7497,7 +7509,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A16" s="21" t="s">
         <v>36</v>
       </c>
@@ -7520,7 +7532,7 @@
       </c>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A17" s="21" t="s">
         <v>38</v>
       </c>
@@ -7545,7 +7557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="21" t="s">
         <v>39</v>
       </c>
@@ -7564,7 +7576,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A16:C16"/>

</xml_diff>

<commit_message>
Added Monique as a discussant again
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Phd\Jobs\Apec seminar\apecseminar.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C8ED81-CB0E-4137-904F-CCF1AF73B492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF61D6F-E592-42B1-9C43-4AF4353067C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="MS Symposium" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="235">
   <si>
     <t>Date</t>
   </si>
@@ -4741,12 +4741,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="20.76953125" customWidth="1"/>
+    <col min="1" max="8" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>117</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="59" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
@@ -4808,7 +4808,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10"/>
@@ -4817,7 +4817,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10"/>
@@ -4829,7 +4829,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10"/>
@@ -4841,7 +4841,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="10"/>
@@ -4850,7 +4850,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10"/>
@@ -4859,7 +4859,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
@@ -4868,7 +4868,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
@@ -4877,7 +4877,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
@@ -4886,7 +4886,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="10"/>
@@ -4895,7 +4895,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="10"/>
@@ -4904,7 +4904,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="10"/>
@@ -4913,7 +4913,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="10"/>
@@ -4922,7 +4922,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="10"/>
@@ -4931,7 +4931,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
+    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A17:C17"/>
@@ -5014,27 +5014,27 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.2265625" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.2265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.6796875" customWidth="1"/>
-    <col min="20" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.21875" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.6640625" customWidth="1"/>
+    <col min="20" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>123</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>124</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>126</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>127</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="N7">
         <v>5</v>
@@ -5169,7 +5169,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N11">
         <v>9</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N12">
         <v>10</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N13">
         <v>11</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N14">
         <v>12</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N15">
         <v>13</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N16">
         <v>14</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="17" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N17">
         <v>15</v>
       </c>
@@ -5356,17 +5356,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="19" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N19" s="20" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="21" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N21" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="22" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N22" t="s">
         <v>146</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="23" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N23">
         <f>1+1+1+1+1</f>
         <v>5</v>
@@ -5391,7 +5391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="24" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N24" s="16">
         <f>N23/SUM($N$23:$P$23)</f>
         <v>0.38461538461538464</v>
@@ -5405,12 +5405,12 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="26" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="26" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="27" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N27" t="s">
         <v>157</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="28" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N28">
         <f>1+1+1+1+1+1+1</f>
         <v>7</v>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="29" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N29" s="16">
         <f t="shared" ref="N29:Z29" si="0">N28/SUM($N$28:$Z$28)</f>
         <v>0.2413793103448276</v>
@@ -5573,26 +5573,26 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.2265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.31640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.31640625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.86328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5546875" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.86328125" style="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>173</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>174</v>
       </c>
@@ -5787,7 +5787,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="59" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>175</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>176</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>177</v>
       </c>
@@ -5873,6 +5873,9 @@
       </c>
       <c r="E8" s="17" t="s">
         <v>196</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
@@ -5889,7 +5892,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>178</v>
       </c>
@@ -5923,7 +5926,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>179</v>
       </c>
@@ -5954,7 +5957,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>180</v>
       </c>
@@ -5985,7 +5988,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>181</v>
       </c>
@@ -6016,7 +6019,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -6050,7 +6053,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>183</v>
       </c>
@@ -6084,7 +6087,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>184</v>
       </c>
@@ -6118,7 +6121,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>185</v>
       </c>
@@ -6149,7 +6152,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -6172,7 +6175,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -6197,7 +6200,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -6216,43 +6219,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C25" s="17"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C26" s="17"/>
       <c r="D26" s="18"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C27" s="17"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C31" s="17"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C32" s="17"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="17"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" s="17"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" s="17"/>
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" s="17"/>
       <c r="D36" s="18"/>
     </row>
@@ -6275,21 +6278,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.2265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="8" customWidth="1"/>
-    <col min="4" max="4" width="45.76953125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.6796875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.2265625" customWidth="1"/>
-    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.54296875" customWidth="1"/>
+    <col min="4" max="4" width="45.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6324,7 +6327,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="59" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -6358,7 +6361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -6392,7 +6395,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -6426,7 +6429,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -6463,7 +6466,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -6497,7 +6500,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -6534,7 +6537,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="27.25" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -6568,7 +6571,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
@@ -6605,7 +6608,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -6639,7 +6642,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -6676,7 +6679,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -6713,7 +6716,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -6747,7 +6750,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27.25" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -6781,7 +6784,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
@@ -6818,7 +6821,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -6852,7 +6855,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -6875,7 +6878,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -6900,7 +6903,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -6919,29 +6922,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E29"/>
     </row>
   </sheetData>
@@ -6963,21 +6966,21 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.2265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.31640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.31640625" customWidth="1"/>
-    <col min="5" max="5" width="15.31640625" customWidth="1"/>
-    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -7012,7 +7015,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="59" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -7046,7 +7049,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -7083,7 +7086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -7117,7 +7120,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -7151,7 +7154,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -7188,7 +7191,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -7225,7 +7228,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -7262,7 +7265,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -7299,7 +7302,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -7336,7 +7339,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -7370,7 +7373,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -7407,7 +7410,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -7441,7 +7444,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -7475,7 +7478,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -7509,7 +7512,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>36</v>
       </c>
@@ -7532,7 +7535,7 @@
       </c>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>38</v>
       </c>
@@ -7557,7 +7560,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>39</v>
       </c>
@@ -7576,7 +7579,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
+    <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A16:C16"/>

</xml_diff>

<commit_message>
Updated attendance for Willy workshop
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF61D6F-E592-42B1-9C43-4AF4353067C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0171B9E5-8776-4BE6-AD32-22034F8A33DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -1118,34 +1118,34 @@
                   <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>76</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="Q8">
         <f>'2024 - Fall'!K7</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="Q9">
         <f>'2024 - Fall'!K8</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="Q10">
         <f>'2024 - Fall'!K9</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -5255,7 +5255,7 @@
       </c>
       <c r="Q11">
         <f>'2024 - Fall'!K10</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -5272,7 +5272,7 @@
       </c>
       <c r="Q12">
         <f>'2024 - Fall'!K11</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5323,7 +5323,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.3">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
@@ -5573,7 +5573,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5843,16 +5843,22 @@
       <c r="F7" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="G7" s="1">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1">
+        <v>10</v>
+      </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s">
         <v>225</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>233</v>
@@ -5886,7 +5892,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>234</v>
@@ -5920,7 +5926,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>234</v>
@@ -5951,7 +5957,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>233</v>
@@ -5982,7 +5988,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>234</v>
@@ -6013,7 +6019,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>234</v>
@@ -6047,7 +6053,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>233</v>
@@ -6081,7 +6087,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>233</v>
@@ -6115,7 +6121,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>234</v>
@@ -6146,7 +6152,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>234</v>
@@ -6163,15 +6169,15 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6186,15 +6192,15 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>9.8000000000000007</v>
+        <v>9.3333333333333339</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>5.4</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>15.200000000000001</v>
+        <v>15.5</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6213,7 +6219,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.2</v>
+        <v>0.20394736842105263</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added nobel pick competition to social.qmd
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0171B9E5-8776-4BE6-AD32-22034F8A33DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BA5972-FADD-478B-B7B1-51A20178AC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -5572,8 +5572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updating with the seminar of Oct 16th
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Phd\Jobs\Apec seminar\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BA5972-FADD-478B-B7B1-51A20178AC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A22543A-801D-404C-A849-3F986DDA213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="MS Symposium" sheetId="3" r:id="rId1"/>
@@ -1121,31 +1121,31 @@
                   <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>93</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4741,12 +4741,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="8" width="20.77734375" customWidth="1"/>
+    <col min="1" max="8" width="20.76953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>117</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="59" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
@@ -4808,7 +4808,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10"/>
@@ -4817,7 +4817,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10"/>
@@ -4829,7 +4829,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10"/>
@@ -4841,7 +4841,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="10"/>
@@ -4850,7 +4850,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10"/>
@@ -4859,7 +4859,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
@@ -4868,7 +4868,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
@@ -4877,7 +4877,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
@@ -4886,7 +4886,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="10"/>
@@ -4895,7 +4895,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="10"/>
@@ -4904,7 +4904,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="10"/>
@@ -4913,7 +4913,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="10"/>
@@ -4922,7 +4922,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="10"/>
@@ -4931,7 +4931,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:8" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A17:C17"/>
@@ -5017,24 +5017,24 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" customWidth="1"/>
-    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.6640625" customWidth="1"/>
-    <col min="20" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.2265625" customWidth="1"/>
+    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.2265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.6796875" customWidth="1"/>
+    <col min="20" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A1" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A3" s="13" t="s">
         <v>123</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A4" s="13" t="s">
         <v>124</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A5" s="13" t="s">
         <v>126</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A6" s="13" t="s">
         <v>127</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A7" s="14"/>
       <c r="N7">
         <v>5</v>
@@ -5169,7 +5169,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -5214,10 +5214,10 @@
       </c>
       <c r="Q9">
         <f>'2024 - Fall'!K8</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.75">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -5238,10 +5238,10 @@
       </c>
       <c r="Q10">
         <f>'2024 - Fall'!K9</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N11">
         <v>9</v>
       </c>
@@ -5255,10 +5255,10 @@
       </c>
       <c r="Q11">
         <f>'2024 - Fall'!K10</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N12">
         <v>10</v>
       </c>
@@ -5272,10 +5272,10 @@
       </c>
       <c r="Q12">
         <f>'2024 - Fall'!K11</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N13">
         <v>11</v>
       </c>
@@ -5289,10 +5289,10 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N14">
         <v>12</v>
       </c>
@@ -5306,10 +5306,10 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N15">
         <v>13</v>
       </c>
@@ -5323,10 +5323,10 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.75">
       <c r="N16">
         <v>14</v>
       </c>
@@ -5340,10 +5340,10 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="14:26" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N17">
         <v>15</v>
       </c>
@@ -5353,20 +5353,20 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="14:26" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N19" s="20" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N21" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N22" t="s">
         <v>146</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N23">
         <f>1+1+1+1+1</f>
         <v>5</v>
@@ -5391,7 +5391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N24" s="16">
         <f>N23/SUM($N$23:$P$23)</f>
         <v>0.38461538461538464</v>
@@ -5405,12 +5405,12 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="26" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N26" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N27" t="s">
         <v>157</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N28">
         <f>1+1+1+1+1+1+1</f>
         <v>7</v>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="14:26" x14ac:dyDescent="0.75">
       <c r="N29" s="16">
         <f t="shared" ref="N29:Z29" si="0">N28/SUM($N$28:$Z$28)</f>
         <v>0.2413793103448276</v>
@@ -5572,27 +5572,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.2265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.31640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.31640625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.86328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5630,7 +5628,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -5667,7 +5665,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -5707,7 +5705,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>173</v>
       </c>
@@ -5747,7 +5745,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>174</v>
       </c>
@@ -5787,7 +5785,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="59" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>175</v>
       </c>
@@ -5824,7 +5822,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>176</v>
       </c>
@@ -5864,7 +5862,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>177</v>
       </c>
@@ -5883,22 +5881,28 @@
       <c r="F8" s="17" t="s">
         <v>89</v>
       </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>6</v>
+      </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J8" t="s">
         <v>227</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>178</v>
       </c>
@@ -5926,13 +5930,13 @@
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>179</v>
       </c>
@@ -5957,13 +5961,13 @@
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>180</v>
       </c>
@@ -5988,13 +5992,13 @@
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>181</v>
       </c>
@@ -6019,13 +6023,13 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -6053,13 +6057,13 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>183</v>
       </c>
@@ -6087,13 +6091,13 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>184</v>
       </c>
@@ -6121,13 +6125,13 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>185</v>
       </c>
@@ -6152,13 +6156,13 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -6169,19 +6173,19 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -6192,21 +6196,21 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>9.3333333333333339</v>
+        <v>8.5714285714285712</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>6.166666666666667</v>
+        <v>6.1428571428571432</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>15.5</v>
+        <v>14.714285714285715</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -6219,49 +6223,49 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.20394736842105263</v>
+        <v>0.19360902255639098</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C25" s="17"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C26" s="17"/>
       <c r="D26" s="18"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C27" s="17"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C31" s="17"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.75">
       <c r="C32" s="17"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C33" s="17"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C34" s="17"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C35" s="17"/>
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.75">
       <c r="C36" s="17"/>
       <c r="D36" s="18"/>
     </row>
@@ -6284,21 +6288,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.2265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="8" customWidth="1"/>
-    <col min="4" max="4" width="45.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="4" max="4" width="45.76953125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.6796875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.2265625" customWidth="1"/>
+    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6333,7 +6337,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="59" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -6367,7 +6371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -6401,7 +6405,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -6435,7 +6439,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -6472,7 +6476,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -6506,7 +6510,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -6543,7 +6547,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="27.25" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -6577,7 +6581,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
@@ -6614,7 +6618,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -6648,7 +6652,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -6685,7 +6689,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -6722,7 +6726,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -6756,7 +6760,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="27.25" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -6790,7 +6794,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
@@ -6827,7 +6831,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -6861,7 +6865,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -6884,7 +6888,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -6909,7 +6913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -6928,29 +6932,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
       <c r="E29"/>
     </row>
   </sheetData>
@@ -6972,21 +6976,21 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.2265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.31640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.31640625" customWidth="1"/>
+    <col min="5" max="5" width="15.31640625" customWidth="1"/>
+    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -7021,7 +7025,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="59" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -7055,7 +7059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -7092,7 +7096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -7126,7 +7130,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -7160,7 +7164,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -7197,7 +7201,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -7234,7 +7238,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -7271,7 +7275,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -7308,7 +7312,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -7345,7 +7349,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -7379,7 +7383,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -7416,7 +7420,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -7450,7 +7454,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -7484,7 +7488,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -7518,7 +7522,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A16" s="21" t="s">
         <v>36</v>
       </c>
@@ -7541,7 +7545,7 @@
       </c>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A17" s="21" t="s">
         <v>38</v>
       </c>
@@ -7566,7 +7570,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="21" t="s">
         <v>39</v>
       </c>
@@ -7585,7 +7589,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A16:C16"/>

</xml_diff>

<commit_message>
Updating with Caroline Krafft workshop
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Phd\Jobs\Apec seminar\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A22543A-801D-404C-A849-3F986DDA213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7382D091-07DA-4091-9500-0D5789B7EFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -1124,28 +1124,28 @@
                   <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>103</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>103</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>103</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>103</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>103</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>103</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>103</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>103</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="Q10">
         <f>'2024 - Fall'!K9</f>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.75">
@@ -5255,7 +5255,7 @@
       </c>
       <c r="Q11">
         <f>'2024 - Fall'!K10</f>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.75">
@@ -5272,7 +5272,7 @@
       </c>
       <c r="Q12">
         <f>'2024 - Fall'!K11</f>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.75">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.75">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.75">
@@ -5323,7 +5323,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.75">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.75">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.75">
@@ -5572,7 +5572,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
@@ -5921,16 +5923,22 @@
       <c r="F9" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>9</v>
+      </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J9" t="s">
         <v>228</v>
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>234</v>
@@ -5961,7 +5969,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>233</v>
@@ -5992,7 +6000,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>234</v>
@@ -6023,7 +6031,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>234</v>
@@ -6057,7 +6065,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>233</v>
@@ -6091,7 +6099,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>233</v>
@@ -6125,7 +6133,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>234</v>
@@ -6156,7 +6164,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>234</v>
@@ -6173,15 +6181,15 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6196,15 +6204,15 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>8.5714285714285712</v>
+        <v>8</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>6.1428571428571432</v>
+        <v>6.5</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>14.714285714285715</v>
+        <v>14.5</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6223,7 +6231,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.19360902255639098</v>
+        <v>0.19078947368421054</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added slides for Caroline Krafft
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Drive\Phd\Jobs\Apec seminar\apecseminar.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A22543A-801D-404C-A849-3F986DDA213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499A1D33-211D-4BD5-BB52-558F29373A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="MS Symposium" sheetId="3" r:id="rId1"/>
@@ -4741,12 +4741,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="20.76953125" customWidth="1"/>
+    <col min="1" max="8" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>117</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="59" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
@@ -4808,7 +4808,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10"/>
@@ -4817,7 +4817,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10"/>
@@ -4829,7 +4829,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10"/>
@@ -4841,7 +4841,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="10"/>
@@ -4850,7 +4850,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10"/>
@@ -4859,7 +4859,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
@@ -4868,7 +4868,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
@@ -4877,7 +4877,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
@@ -4886,7 +4886,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="10"/>
@@ -4895,7 +4895,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="10"/>
@@ -4904,7 +4904,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="10"/>
@@ -4913,7 +4913,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="10"/>
@@ -4922,7 +4922,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="10"/>
@@ -4931,7 +4931,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
+    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A17:C17"/>
@@ -5017,24 +5017,24 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.2265625" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.2265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.6796875" customWidth="1"/>
-    <col min="20" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.21875" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.6640625" customWidth="1"/>
+    <col min="20" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>123</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>124</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>126</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>127</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="N7">
         <v>5</v>
@@ -5169,7 +5169,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -5217,7 +5217,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N11">
         <v>9</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N12">
         <v>10</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N13">
         <v>11</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N14">
         <v>12</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N15">
         <v>13</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="N16">
         <v>14</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="17" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N17">
         <v>15</v>
       </c>
@@ -5356,17 +5356,17 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="19" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N19" s="20" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="21" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="21" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N21" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="22" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N22" t="s">
         <v>146</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="23" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N23">
         <f>1+1+1+1+1</f>
         <v>5</v>
@@ -5391,7 +5391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="24" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N24" s="16">
         <f>N23/SUM($N$23:$P$23)</f>
         <v>0.38461538461538464</v>
@@ -5405,12 +5405,12 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="26" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="26" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="27" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N27" t="s">
         <v>157</v>
       </c>
@@ -5451,7 +5451,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="28" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N28">
         <f>1+1+1+1+1+1+1</f>
         <v>7</v>
@@ -5505,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="14:26" x14ac:dyDescent="0.75">
+    <row r="29" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N29" s="16">
         <f t="shared" ref="N29:Z29" si="0">N28/SUM($N$28:$Z$28)</f>
         <v>0.2413793103448276</v>
@@ -5572,25 +5572,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.2265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.31640625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.31640625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.86328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5546875" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.86328125" style="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5628,7 +5630,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>171</v>
       </c>
@@ -5665,7 +5667,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>172</v>
       </c>
@@ -5705,7 +5707,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>173</v>
       </c>
@@ -5745,7 +5747,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>174</v>
       </c>
@@ -5785,7 +5787,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="59" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>175</v>
       </c>
@@ -5822,7 +5824,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>176</v>
       </c>
@@ -5862,7 +5864,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>177</v>
       </c>
@@ -5902,7 +5904,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>178</v>
       </c>
@@ -5936,7 +5938,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>179</v>
       </c>
@@ -5967,7 +5969,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>180</v>
       </c>
@@ -5998,7 +6000,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>181</v>
       </c>
@@ -6029,7 +6031,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -6063,7 +6065,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>183</v>
       </c>
@@ -6097,7 +6099,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>184</v>
       </c>
@@ -6131,7 +6133,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>185</v>
       </c>
@@ -6162,7 +6164,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -6185,7 +6187,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -6210,7 +6212,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -6229,43 +6231,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C25" s="17"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C26" s="17"/>
       <c r="D26" s="18"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C27" s="17"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C31" s="17"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C32" s="17"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="17"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" s="17"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" s="17"/>
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.75">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" s="17"/>
       <c r="D36" s="18"/>
     </row>
@@ -6288,21 +6290,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.2265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="8" customWidth="1"/>
-    <col min="4" max="4" width="45.76953125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.6796875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.2265625" customWidth="1"/>
-    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.54296875" customWidth="1"/>
+    <col min="4" max="4" width="45.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6337,7 +6339,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="59" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -6371,7 +6373,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -6405,7 +6407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -6439,7 +6441,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -6476,7 +6478,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -6510,7 +6512,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -6547,7 +6549,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="27.25" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -6581,7 +6583,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
@@ -6618,7 +6620,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -6652,7 +6654,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -6689,7 +6691,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -6726,7 +6728,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -6760,7 +6762,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27.25" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -6794,7 +6796,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
@@ -6831,7 +6833,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -6865,7 +6867,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>36</v>
       </c>
@@ -6888,7 +6890,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
@@ -6913,7 +6915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
@@ -6932,29 +6934,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E29"/>
     </row>
   </sheetData>
@@ -6976,21 +6978,21 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.2265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.31640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.31640625" customWidth="1"/>
-    <col min="5" max="5" width="15.31640625" customWidth="1"/>
-    <col min="6" max="6" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.76953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.54296875" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -7025,7 +7027,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="59" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -7059,7 +7061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -7096,7 +7098,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -7130,7 +7132,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -7164,7 +7166,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -7201,7 +7203,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -7238,7 +7240,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -7275,7 +7277,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -7312,7 +7314,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -7349,7 +7351,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -7383,7 +7385,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -7420,7 +7422,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -7454,7 +7456,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -7488,7 +7490,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="44.25" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -7522,7 +7524,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="21" t="s">
         <v>36</v>
       </c>
@@ -7545,7 +7547,7 @@
       </c>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>38</v>
       </c>
@@ -7570,7 +7572,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="16.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.9">
+    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21" t="s">
         <v>39</v>
       </c>
@@ -7589,7 +7591,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.5" thickTop="1" x14ac:dyDescent="0.75"/>
+    <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A16:C16"/>

</xml_diff>

<commit_message>
Added Noah Wexler as discussant to attendance sheet
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77B9036-2862-426E-8642-3636FF0DD232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9DBFD5-CEA4-482E-8FF9-62D28BC6F37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="238">
   <si>
     <t>Date</t>
   </si>
@@ -598,9 +598,6 @@
   </si>
   <si>
     <t>Dec. 11th</t>
-  </si>
-  <si>
-    <t>Thanksgiving Nov. 28th</t>
   </si>
   <si>
     <t>Lindsey Novak</t>
@@ -762,7 +759,13 @@
     <t>Education, Policy, Discrimination</t>
   </si>
   <si>
-    <t>TBD</t>
+    <t>Noah Wexler</t>
+  </si>
+  <si>
+    <t>JMC</t>
+  </si>
+  <si>
+    <t>Thanksgiving Nov. 28th, JMC</t>
   </si>
 </sst>
 </file>
@@ -5058,7 +5061,7 @@
         <v>118</v>
       </c>
       <c r="Q2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -5364,7 +5367,7 @@
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
       <c r="N19" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="14:26" x14ac:dyDescent="0.3">
@@ -5578,8 +5581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5633,7 +5636,7 @@
         <v>128</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -5647,10 +5650,10 @@
         <v>53</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>50</v>
@@ -5665,12 +5668,15 @@
         <f t="shared" ref="I2:I16" si="0">SUM(G2:H2)</f>
         <v>16</v>
       </c>
+      <c r="J2" t="s">
+        <v>236</v>
+      </c>
       <c r="K2">
         <f>I2</f>
         <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -5681,10 +5687,10 @@
         <v>83</v>
       </c>
       <c r="C3" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>212</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>146</v>
@@ -5710,7 +5716,7 @@
         <v>38</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -5721,13 +5727,13 @@
         <v>33</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>61</v>
@@ -5750,7 +5756,7 @@
         <v>53</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -5761,10 +5767,10 @@
         <v>83</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>214</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>146</v>
@@ -5783,14 +5789,14 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
@@ -5801,13 +5807,13 @@
         <v>33</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>93</v>
@@ -5822,12 +5828,15 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="J6" t="s">
+        <v>236</v>
+      </c>
       <c r="K6">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -5838,13 +5847,13 @@
         <v>83</v>
       </c>
       <c r="C7" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="17" t="s">
         <v>216</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>217</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>61</v>
@@ -5860,14 +5869,14 @@
         <v>17</v>
       </c>
       <c r="J7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -5878,13 +5887,13 @@
         <v>33</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>89</v>
@@ -5900,14 +5909,14 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -5918,10 +5927,10 @@
         <v>83</v>
       </c>
       <c r="C9" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>219</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>146</v>
@@ -5940,14 +5949,14 @@
         <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -5958,27 +5967,30 @@
         <v>33</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J10" t="s">
+        <v>236</v>
+      </c>
       <c r="K10">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -5992,24 +6004,27 @@
         <v>89</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="F11" s="17" t="s">
         <v>235</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>236</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J11" t="s">
+        <v>236</v>
+      </c>
       <c r="K11">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -6020,27 +6035,30 @@
         <v>33</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E12" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J12" t="s">
+        <v>236</v>
+      </c>
       <c r="K12">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -6051,10 +6069,10 @@
         <v>83</v>
       </c>
       <c r="C13" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>220</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>221</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>147</v>
@@ -6067,14 +6085,14 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -6088,10 +6106,10 @@
         <v>99</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>85</v>
@@ -6101,14 +6119,14 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>186</v>
+        <v>237</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -6119,13 +6137,13 @@
         <v>83</v>
       </c>
       <c r="C15" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>223</v>
-      </c>
       <c r="E15" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>61</v>
@@ -6142,7 +6160,7 @@
         <v>117</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -6153,27 +6171,30 @@
         <v>33</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="J16" t="s">
+        <v>236</v>
+      </c>
       <c r="K16">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6297,9 +6318,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9DA028-C994-415A-B404-123C1AD93D08}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6380,6 +6401,9 @@
         <f t="shared" ref="I2:I16" si="0">SUM(G2:H2)</f>
         <v>10</v>
       </c>
+      <c r="J2" t="s">
+        <v>236</v>
+      </c>
       <c r="K2">
         <f>I2</f>
         <v>10</v>
@@ -6414,6 +6438,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="J3" t="s">
+        <v>236</v>
+      </c>
       <c r="K3">
         <f t="shared" ref="K3:K16" si="1">K2+I3</f>
         <v>21</v>
@@ -6519,6 +6546,9 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
+      <c r="J6" t="s">
+        <v>236</v>
+      </c>
       <c r="K6">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -6661,6 +6691,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="J10" t="s">
+        <v>236</v>
+      </c>
       <c r="K10">
         <f t="shared" si="1"/>
         <v>132</v>
@@ -6802,6 +6835,9 @@
       <c r="I14" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>236</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
@@ -6986,8 +7022,8 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7068,6 +7104,9 @@
         <f t="shared" ref="I2:I17" si="0">SUM(G2:H2)</f>
         <v>10</v>
       </c>
+      <c r="J2" t="s">
+        <v>236</v>
+      </c>
       <c r="K2">
         <f>I2</f>
         <v>10</v>
@@ -7139,6 +7178,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="J4" t="s">
+        <v>236</v>
+      </c>
       <c r="K4">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -7392,6 +7434,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="J11" t="s">
+        <v>236</v>
+      </c>
       <c r="K11">
         <f t="shared" si="1"/>
         <v>158</v>
@@ -7497,6 +7542,9 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
+      <c r="J14" t="s">
+        <v>236</v>
+      </c>
       <c r="K14">
         <f t="shared" si="1"/>
         <v>204</v>
@@ -7530,6 +7578,9 @@
       <c r="I15" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>236</v>
       </c>
       <c r="K15">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Changes to seminar organizer assignments
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3D037A-A35C-4D8F-96EF-7C79CDA255BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56BF5C4-4E1A-4AB8-B1BC-715170704195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -5569,8 +5569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6018,7 +6018,7 @@
         <v>126</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -6120,7 +6120,7 @@
         <v>126</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added attendance for Monique presentation
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56BF5C4-4E1A-4AB8-B1BC-715170704195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F84870-ACE0-44BC-986B-93A5D1FAC031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="237">
   <si>
     <t>Date</t>
   </si>
@@ -760,6 +760,9 @@
   </si>
   <si>
     <t>Thanksgiving Nov. 28th, JMC</t>
+  </si>
+  <si>
+    <t>JMC, Day after 2024 Election</t>
   </si>
 </sst>
 </file>
@@ -1133,22 +1136,22 @@
                   <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>126</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>126</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>126</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>126</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>126</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>126</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5269,7 +5272,7 @@
       </c>
       <c r="Q12">
         <f>'2024 - Fall'!K11</f>
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -5286,7 +5289,7 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5303,7 +5306,7 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5320,7 +5323,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5337,7 +5340,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.3">
@@ -5350,7 +5353,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>126</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
@@ -5570,7 +5573,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6006,16 +6009,22 @@
       <c r="F11" s="17" t="s">
         <v>233</v>
       </c>
+      <c r="G11" s="1">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J11" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>229</v>
@@ -6049,7 +6058,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>230</v>
@@ -6083,7 +6092,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>229</v>
@@ -6117,7 +6126,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>230</v>
@@ -6151,7 +6160,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>230</v>
@@ -6185,7 +6194,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>230</v>
@@ -6202,15 +6211,15 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6225,15 +6234,15 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>8.2222222222222214</v>
+        <v>7.8</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>5.7777777777777777</v>
+        <v>5.5</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>14</v>
+        <v>13.3</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6252,7 +6261,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.18421052631578946</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>
@@ -6313,7 +6322,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated attendance for Qingyin presentation
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F84870-ACE0-44BC-986B-93A5D1FAC031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E8EE24-4AF3-4DEA-B276-963D86E2ADCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -1139,19 +1139,19 @@
                   <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>133</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>133</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>133</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>133</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>133</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5014,7 +5014,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5289,7 +5289,7 @@
       </c>
       <c r="Q13">
         <f>'2024 - Fall'!K12</f>
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5323,7 +5323,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.3">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>133</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
@@ -5572,8 +5572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6049,16 +6049,22 @@
       <c r="F12" s="19" t="s">
         <v>206</v>
       </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>11</v>
+      </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J12" t="s">
         <v>234</v>
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>230</v>
@@ -6092,7 +6098,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>229</v>
@@ -6126,7 +6132,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>230</v>
@@ -6160,7 +6166,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>230</v>
@@ -6194,7 +6200,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>230</v>
@@ -6211,15 +6217,15 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6234,15 +6240,15 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>7.8</v>
+        <v>7.3636363636363633</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>13.3</v>
+        <v>13.363636363636363</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6261,7 +6267,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.17500000000000002</v>
+        <v>0.17583732057416268</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Updated attendance for Redish talk
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E8EE24-4AF3-4DEA-B276-963D86E2ADCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D80FDE-740C-4F91-9F20-222D227C0245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -1142,16 +1142,16 @@
                   <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>147</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>147</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>147</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>147</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5014,7 +5014,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5306,7 +5306,7 @@
       </c>
       <c r="Q14">
         <f>'2024 - Fall'!K13</f>
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -5323,7 +5323,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.3">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
@@ -5572,8 +5572,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6089,16 +6090,22 @@
       <c r="F13" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="G13" s="1">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1">
+        <v>9</v>
+      </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J13" t="s">
         <v>225</v>
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>229</v>
@@ -6132,7 +6139,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>230</v>
@@ -6166,7 +6173,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>230</v>
@@ -6200,7 +6207,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>230</v>
@@ -6217,15 +6224,15 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6240,15 +6247,15 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>7.3636363636363633</v>
+        <v>7.5</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>13.363636363636363</v>
+        <v>13.75</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6267,7 +6274,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.17583732057416268</v>
+        <v>0.18092105263157895</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added attendance for Yanxu presentation
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D80FDE-740C-4F91-9F20-222D227C0245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA82DCB9-C377-403F-B6FA-0C02BA8F9A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-20760" yWindow="3300" windowWidth="17280" windowHeight="8970" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="MS Symposium" sheetId="3" r:id="rId1"/>
@@ -1145,13 +1145,13 @@
                   <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>165</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>165</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>165</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5323,7 +5323,7 @@
       </c>
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="Q16">
         <f>'2024 - Fall'!K15</f>
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="14:26" x14ac:dyDescent="0.3">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="Q17">
         <f>'2024 - Fall'!K16</f>
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="14:26" x14ac:dyDescent="0.3">
@@ -5573,8 +5573,8 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6130,16 +6130,22 @@
       <c r="F14" s="17" t="s">
         <v>85</v>
       </c>
+      <c r="G14" s="1">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>6</v>
+      </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J14" t="s">
         <v>235</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>230</v>
@@ -6173,7 +6179,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>230</v>
@@ -6207,7 +6213,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="1"/>
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>230</v>
@@ -6224,15 +6230,15 @@
       <c r="F17" s="11"/>
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(G17:H17)</f>
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -6247,15 +6253,15 @@
       <c r="F18" s="11"/>
       <c r="G18" s="4">
         <f>AVERAGE(G2:G16)</f>
-        <v>7.5</v>
+        <v>7.3076923076923075</v>
       </c>
       <c r="H18" s="4">
         <f>AVERAGE(H2:H16)</f>
-        <v>6.25</v>
+        <v>6.2307692307692308</v>
       </c>
       <c r="I18" s="4">
         <f>SUM(G18:H18)</f>
-        <v>13.75</v>
+        <v>13.538461538461538</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>40</v>
@@ -6274,7 +6280,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="6">
         <f>I18/(64+12)</f>
-        <v>0.18092105263157895</v>
+        <v>0.17813765182186234</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Added Spring 2025 to attendance sheet
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFC1985-D763-4284-9849-69E7F71BF169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD710D7-7031-4297-B095-F150BF41561B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="769" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="MS Symposium" sheetId="3" r:id="rId1"/>
     <sheet name="Attendance Descriptives" sheetId="4" r:id="rId2"/>
-    <sheet name="2024 - Fall" sheetId="5" r:id="rId3"/>
-    <sheet name="2024 - Spring" sheetId="2" r:id="rId4"/>
-    <sheet name="2023 - Fall" sheetId="1" r:id="rId5"/>
+    <sheet name="2025 - Spring" sheetId="6" r:id="rId3"/>
+    <sheet name="2024 - Fall" sheetId="5" r:id="rId4"/>
+    <sheet name="2024 - Spring" sheetId="2" r:id="rId5"/>
+    <sheet name="2023 - Fall" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="256">
   <si>
     <t>Date</t>
   </si>
@@ -764,12 +765,69 @@
   <si>
     <t>JMC, Day after 2024 Election</t>
   </si>
+  <si>
+    <t>Spring 2025</t>
+  </si>
+  <si>
+    <t>Jan. 22nd</t>
+  </si>
+  <si>
+    <t>Jan. 29th</t>
+  </si>
+  <si>
+    <t>Feb. 5th</t>
+  </si>
+  <si>
+    <t>Feb. 12th</t>
+  </si>
+  <si>
+    <t>Feb. 19th</t>
+  </si>
+  <si>
+    <t>Mar. 5th</t>
+  </si>
+  <si>
+    <t>Neural Correlates of visual attention and its correlation with consumer preferences using eye-tracking and EEG</t>
+  </si>
+  <si>
+    <t>Uma Parasuram</t>
+  </si>
+  <si>
+    <t>Runcheng Xu</t>
+  </si>
+  <si>
+    <t>Reflections on the Job Market</t>
+  </si>
+  <si>
+    <t>Ling Yao, Monique Davis, …</t>
+  </si>
+  <si>
+    <t>Ryan McWay</t>
+  </si>
+  <si>
+    <t>Using the Bartik Instrument Variable (Shift-share IV)</t>
+  </si>
+  <si>
+    <t>Teaching as a Graduate Student</t>
+  </si>
+  <si>
+    <t>Fieldwork Management and Data Collection</t>
+  </si>
+  <si>
+    <t>Doubly Robust Estimators and Covariate Selection</t>
+  </si>
+  <si>
+    <t>Paul Glewwe</t>
+  </si>
+  <si>
+    <t>Raahil Madock</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -795,6 +853,19 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -861,7 +932,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -913,6 +984,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1007,8 +1080,153 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Spring 2025</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-EBBD-48AB-8F7C-852FCD068F84}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="LM Roman 12" panose="00000500000000000000" pitchFamily="50" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Attendance Descriptives'!$R$3:$R$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EBBD-48AB-8F7C-852FCD068F84}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="2"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'Attendance Descriptives'!$Q$2</c:f>
@@ -1165,7 +1383,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'Attendance Descriptives'!$P$2</c:f>
@@ -1320,7 +1538,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>'Attendance Descriptives'!$O$2</c:f>
@@ -5013,8 +5231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A92331-1E38-48FD-9605-0D81D4E71360}">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5027,14 +5245,14 @@
     <col min="20" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -5054,8 +5272,11 @@
       <c r="Q2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>123</v>
       </c>
@@ -5078,8 +5299,12 @@
         <f>'2024 - Fall'!K2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <f>'2025 - Spring'!K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>124</v>
       </c>
@@ -5102,8 +5327,12 @@
         <f>'2024 - Fall'!K3</f>
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <f>'2025 - Spring'!K3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>126</v>
       </c>
@@ -5126,8 +5355,12 @@
         <f>'2024 - Fall'!K4</f>
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <f>'2025 - Spring'!K4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>127</v>
       </c>
@@ -5150,8 +5383,12 @@
         <f>'2024 - Fall'!K5</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <f>'2025 - Spring'!K5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="N7">
         <v>5</v>
@@ -5168,8 +5405,12 @@
         <f>'2024 - Fall'!K6</f>
         <v>76</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <f>'2025 - Spring'!K6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
@@ -5192,8 +5433,12 @@
         <f>'2024 - Fall'!K7</f>
         <v>93</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <f>'2025 - Spring'!K7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -5216,8 +5461,12 @@
         <f>'2024 - Fall'!K8</f>
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <f>'2025 - Spring'!K8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -5240,8 +5489,12 @@
         <f>'2024 - Fall'!K9</f>
         <v>117</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10">
+        <f>'2025 - Spring'!K9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N11">
         <v>9</v>
       </c>
@@ -5257,8 +5510,12 @@
         <f>'2024 - Fall'!K10</f>
         <v>126</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <f>'2025 - Spring'!K10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N12">
         <v>10</v>
       </c>
@@ -5274,8 +5531,12 @@
         <f>'2024 - Fall'!K11</f>
         <v>133</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <f>'2025 - Spring'!K11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N13">
         <v>11</v>
       </c>
@@ -5291,8 +5552,12 @@
         <f>'2024 - Fall'!K12</f>
         <v>147</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <f>'2025 - Spring'!K12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N14">
         <v>12</v>
       </c>
@@ -5308,8 +5573,12 @@
         <f>'2024 - Fall'!K13</f>
         <v>165</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14">
+        <f>'2025 - Spring'!K13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N15">
         <v>13</v>
       </c>
@@ -5325,8 +5594,12 @@
         <f>'2024 - Fall'!K14</f>
         <v>176</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <f>'2025 - Spring'!K14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N16">
         <v>14</v>
       </c>
@@ -5569,12 +5842,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
-  <dimension ref="A1:L36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0179C6-09EB-4EF2-AC44-670A4027DE80}">
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5631,6 +5903,471 @@
         <v>228</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="F2" s="19"/>
+      <c r="I2" s="1">
+        <f t="shared" ref="I2:I14" si="0">SUM(G2:H2)</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>I2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" t="s">
+        <v>250</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K14" si="1">K2+I3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>251</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" t="s">
+        <v>252</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="F10" s="19"/>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>253</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="17"/>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="2">
+        <f>SUM(G2:G14)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <f>SUM(H2:H14)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <f>SUM(G15:H15)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="4" t="e">
+        <f>AVERAGE(G2:G14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="4" t="e">
+        <f>AVERAGE(H2:H14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I16" s="4" t="e">
+        <f>SUM(G16:H16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="6" t="e">
+        <f>I16/(64+12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C26" s="17"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C27" s="17"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C28" s="17"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C30" s="17"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C32" s="17"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="17"/>
+      <c r="D33" s="18"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
+  <dimension ref="A1:L36"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
     <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>169</v>
@@ -6348,13 +7085,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9DA028-C994-415A-B404-123C1AD93D08}">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6858,7 +7595,7 @@
         <v>143</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>249</v>
       </c>
       <c r="G14" s="1">
         <v>13</v>
@@ -7051,7 +7788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9118A8-9298-41B4-A7AA-F0BC3EEE1EAD}">
   <dimension ref="A1:K19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated seminar attendance to delete seminar from last week.
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD710D7-7031-4297-B095-F150BF41561B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921386F9-72CC-4CBC-A668-CFF28BA1FE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="769" activeTab="2" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" activeTab="1" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
-    <sheet name="MS Symposium" sheetId="3" r:id="rId1"/>
-    <sheet name="Attendance Descriptives" sheetId="4" r:id="rId2"/>
-    <sheet name="2025 - Spring" sheetId="6" r:id="rId3"/>
-    <sheet name="2024 - Fall" sheetId="5" r:id="rId4"/>
-    <sheet name="2024 - Spring" sheetId="2" r:id="rId5"/>
-    <sheet name="2023 - Fall" sheetId="1" r:id="rId6"/>
+    <sheet name="Attendance Descriptives" sheetId="4" r:id="rId1"/>
+    <sheet name="2025 - Spring" sheetId="6" r:id="rId2"/>
+    <sheet name="2024 - Fall" sheetId="5" r:id="rId3"/>
+    <sheet name="2024 - Spring" sheetId="2" r:id="rId4"/>
+    <sheet name="2023 - Fall" sheetId="1" r:id="rId5"/>
+    <sheet name="MS Symposium" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="255">
   <si>
     <t>Date</t>
   </si>
@@ -767,9 +767,6 @@
   </si>
   <si>
     <t>Spring 2025</t>
-  </si>
-  <si>
-    <t>Jan. 22nd</t>
   </si>
   <si>
     <t>Jan. 29th</t>
@@ -978,14 +975,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1209,9 +1206,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4958,281 +4952,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318A700E-0BF3-43A5-A828-CFE649334312}">
-  <dimension ref="A1:H20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="8" width="20.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G18" si="0">SUM(E2:F2)</f>
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="2">
-        <f>SUM(D2:D16)</f>
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
-        <f>SUM(E2:E16)</f>
-        <v>15</v>
-      </c>
-      <c r="F17" s="2">
-        <f>SUM(F2:F16)</f>
-        <v>4</v>
-      </c>
-      <c r="G17" s="2">
-        <f>SUM(E17:F17)</f>
-        <v>19</v>
-      </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="4">
-        <f>AVERAGE(D2:D16)</f>
-        <v>5</v>
-      </c>
-      <c r="E18" s="4">
-        <f>AVERAGE(E2:E16)</f>
-        <v>15</v>
-      </c>
-      <c r="F18" s="4">
-        <f>AVERAGE(F2:F16)</f>
-        <v>4</v>
-      </c>
-      <c r="G18" s="4">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="6">
-        <f>G18/(64+12)</f>
-        <v>0.25</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A92331-1E38-48FD-9605-0D81D4E71360}">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5246,11 +4970,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -5593,10 +5317,6 @@
       <c r="Q15">
         <f>'2024 - Fall'!K14</f>
         <v>176</v>
-      </c>
-      <c r="R15">
-        <f>'2025 - Spring'!K14</f>
-        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -5841,12 +5561,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0179C6-09EB-4EF2-AC44-670A4027DE80}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5908,42 +5628,47 @@
         <v>238</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="F2" s="19"/>
+        <v>83</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I14" si="0">SUM(G2:H2)</f>
+        <f t="shared" ref="I2:I13" si="0">SUM(G2:H2)</f>
         <v>0</v>
       </c>
       <c r="K2">
         <f>I2</f>
         <v>0</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>239</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>255</v>
-      </c>
-      <c r="D3" t="s">
-        <v>250</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C3" s="17"/>
       <c r="I3" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K14" si="1">K2+I3</f>
+        <f>K2+I3</f>
         <v>0</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -5951,15 +5676,26 @@
         <v>240</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="17"/>
+        <v>83</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K3:K13" si="1">K3+I4</f>
         <v>0</v>
       </c>
     </row>
@@ -5968,14 +5704,11 @@
         <v>241</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>251</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="F5" s="19"/>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5984,6 +5717,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="L5" s="1" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -5993,8 +5729,6 @@
         <v>33</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="F6" s="19"/>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6003,13 +5737,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>243</v>
+        <v>76</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>33</v>
@@ -6026,12 +5757,23 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="17"/>
+        <v>83</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="D8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6040,20 +5782,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="L8" s="1" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>254</v>
-      </c>
-      <c r="D9" t="s">
-        <v>252</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="F9" s="19"/>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6062,19 +5803,26 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="F10" s="19"/>
+        <v>83</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>252</v>
+      </c>
+      <c r="E10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>61</v>
+      </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6083,19 +5831,28 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="L10" s="1" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" t="s">
-        <v>253</v>
+        <v>33</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>245</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
@@ -6106,27 +5863,27 @@
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>245</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>244</v>
+        <v>247</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>246</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>246</v>
+        <v>214</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>248</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
@@ -6140,25 +5897,14 @@
         <v>229</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>248</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>249</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C13" s="17"/>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6167,145 +5913,125 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="I14" s="1">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="2">
+        <f>SUM(G2:G13)</f>
         <v>0</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
+      <c r="H14" s="2">
+        <f>SUM(H2:H13)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
+      <c r="I14" s="2">
+        <f>SUM(G14:H14)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="2">
-        <f>SUM(G2:G14)</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <f>SUM(H2:H14)</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
+      <c r="G15" s="4" t="e">
+        <f>AVERAGE(G2:G13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="4" t="e">
+        <f>AVERAGE(H2:H13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I15" s="4" t="e">
         <f>SUM(G15:H15)</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
+      <c r="A16" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="4" t="e">
-        <f>AVERAGE(G2:G14)</f>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="6" t="e">
+        <f>I15/(64+12)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H16" s="4" t="e">
-        <f>AVERAGE(H2:H14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" s="4" t="e">
-        <f>SUM(G16:H16)</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="J16" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="6" t="e">
-        <f>I16/(64+12)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="17"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" s="17"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="17"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" s="17"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" s="17"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32" s="17"/>
+      <c r="D32" s="18"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" s="17"/>
       <c r="D33" s="18"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEDFB2B-D04A-46F2-AD88-552F372D387B}">
   <dimension ref="A1:L36"/>
   <sheetViews>
@@ -6969,11 +6695,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -6992,11 +6718,11 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -7017,11 +6743,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -7085,7 +6811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9DA028-C994-415A-B404-123C1AD93D08}">
   <dimension ref="A1:K29"/>
   <sheetViews>
@@ -7595,7 +7321,7 @@
         <v>143</v>
       </c>
       <c r="F14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G14" s="1">
         <v>13</v>
@@ -7687,11 +7413,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="2"/>
@@ -7710,11 +7436,11 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="2"/>
@@ -7735,11 +7461,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="2"/>
@@ -7788,7 +7514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9118A8-9298-41B4-A7AA-F0BC3EEE1EAD}">
   <dimension ref="A1:K19"/>
   <sheetViews>
@@ -8359,11 +8085,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -8382,11 +8108,11 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -8407,11 +8133,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -8435,4 +8161,274 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318A700E-0BF3-43A5-A828-CFE649334312}">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="8" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ref="G2:G18" si="0">SUM(E2:F2)</f>
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="2">
+        <f>SUM(D2:D16)</f>
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <f>SUM(E2:E16)</f>
+        <v>15</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(F2:F16)</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="2">
+        <f>SUM(E17:F17)</f>
+        <v>19</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="4">
+        <f>AVERAGE(D2:D16)</f>
+        <v>5</v>
+      </c>
+      <c r="E18" s="4">
+        <f>AVERAGE(E2:E16)</f>
+        <v>15</v>
+      </c>
+      <c r="F18" s="4">
+        <f>AVERAGE(F2:F16)</f>
+        <v>4</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="6">
+        <f>G18/(64+12)</f>
+        <v>0.25</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added attendance for raahil madhok presentation
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921386F9-72CC-4CBC-A668-CFF28BA1FE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730B33E5-5BB9-4823-B64E-92C7A178CBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="769" activeTab="1" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="769" activeTab="1" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance Descriptives" sheetId="4" r:id="rId1"/>
@@ -977,10 +977,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1173,40 +1173,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4970,11 +4970,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="R3">
         <f>'2025 - Spring'!K2</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -5053,7 +5053,7 @@
       </c>
       <c r="R4">
         <f>'2025 - Spring'!K3</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="R5">
         <f>'2025 - Spring'!K4</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -5109,7 +5109,7 @@
       </c>
       <c r="R6">
         <f>'2025 - Spring'!K5</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -5131,7 +5131,7 @@
       </c>
       <c r="R7">
         <f>'2025 - Spring'!K6</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -5159,7 +5159,7 @@
       </c>
       <c r="R8">
         <f>'2025 - Spring'!K7</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -5187,7 +5187,7 @@
       </c>
       <c r="R9">
         <f>'2025 - Spring'!K8</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -5215,7 +5215,7 @@
       </c>
       <c r="R10">
         <f>'2025 - Spring'!K9</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -5236,7 +5236,7 @@
       </c>
       <c r="R11">
         <f>'2025 - Spring'!K10</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="R12">
         <f>'2025 - Spring'!K11</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -5278,7 +5278,7 @@
       </c>
       <c r="R13">
         <f>'2025 - Spring'!K12</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -5299,7 +5299,7 @@
       </c>
       <c r="R14">
         <f>'2025 - Spring'!K13</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -5566,7 +5566,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5642,13 +5642,19 @@
       <c r="F2" s="17" t="s">
         <v>61</v>
       </c>
+      <c r="G2" s="1">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
       <c r="I2" s="1">
         <f t="shared" ref="I2:I13" si="0">SUM(G2:H2)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K2">
         <f>I2</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>229</v>
@@ -5668,7 +5674,7 @@
       </c>
       <c r="K3">
         <f>K2+I3</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -5695,8 +5701,8 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K3:K13" si="1">K3+I4</f>
-        <v>0</v>
+        <f t="shared" ref="K4:K13" si="1">K3+I4</f>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -5715,7 +5721,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>230</v>
@@ -5735,7 +5741,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -5752,7 +5758,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -5780,7 +5786,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>229</v>
@@ -5801,7 +5807,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -5829,7 +5835,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>230</v>
@@ -5860,7 +5866,7 @@
       </c>
       <c r="K11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>229</v>
@@ -5891,7 +5897,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>229</v>
@@ -5911,71 +5917,71 @@
       </c>
       <c r="K13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="2">
         <f>SUM(G2:G13)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H14" s="2">
         <f>SUM(H2:H13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I14" s="2">
         <f>SUM(G14:H14)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="4" t="e">
+      <c r="G15" s="4">
         <f>AVERAGE(G2:G13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="4" t="e">
+        <v>7</v>
+      </c>
+      <c r="H15" s="4">
         <f>AVERAGE(H2:H13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I15" s="4" t="e">
+        <v>4</v>
+      </c>
+      <c r="I15" s="4">
         <f>SUM(G15:H15)</f>
-        <v>#DIV/0!</v>
+        <v>11</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="6" t="e">
+      <c r="I16" s="6">
         <f>I15/(64+12)</f>
-        <v>#DIV/0!</v>
+        <v>0.14473684210526316</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>41</v>
@@ -6695,11 +6701,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -6718,11 +6724,11 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -6743,11 +6749,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -7413,11 +7419,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="2"/>
@@ -7436,11 +7442,11 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="2"/>
@@ -7461,11 +7467,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="2"/>
@@ -8085,11 +8091,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -8108,11 +8114,11 @@
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -8133,11 +8139,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -8356,11 +8362,11 @@
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="2">
         <f>SUM(D2:D16)</f>
         <v>5</v>
@@ -8380,11 +8386,11 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="4">
         <f>AVERAGE(D2:D16)</f>
         <v>5</v>
@@ -8406,11 +8412,11 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="2"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>

</xml_diff>

<commit_message>
Added slides and attendance for paul glewwe workshop
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730B33E5-5BB9-4823-B64E-92C7A178CBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9440103-1F40-4142-A333-EEAA247E32CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="769" activeTab="1" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="251">
   <si>
     <t>Date</t>
   </si>
@@ -772,18 +772,6 @@
     <t>Jan. 29th</t>
   </si>
   <si>
-    <t>Feb. 5th</t>
-  </si>
-  <si>
-    <t>Feb. 12th</t>
-  </si>
-  <si>
-    <t>Feb. 19th</t>
-  </si>
-  <si>
-    <t>Mar. 5th</t>
-  </si>
-  <si>
     <t>Neural Correlates of visual attention and its correlation with consumer preferences using eye-tracking and EEG</t>
   </si>
   <si>
@@ -811,13 +799,13 @@
     <t>Fieldwork Management and Data Collection</t>
   </si>
   <si>
-    <t>Doubly Robust Estimators and Covariate Selection</t>
-  </si>
-  <si>
     <t>Paul Glewwe</t>
   </si>
   <si>
     <t>Raahil Madock</t>
+  </si>
+  <si>
+    <t>Sarah Wahby</t>
   </si>
 </sst>
 </file>
@@ -1176,37 +1164,37 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4956,7 +4944,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5053,7 +5041,7 @@
       </c>
       <c r="R4">
         <f>'2025 - Spring'!K3</f>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -5081,7 +5069,7 @@
       </c>
       <c r="R5">
         <f>'2025 - Spring'!K4</f>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -5109,7 +5097,7 @@
       </c>
       <c r="R6">
         <f>'2025 - Spring'!K5</f>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -5131,7 +5119,7 @@
       </c>
       <c r="R7">
         <f>'2025 - Spring'!K6</f>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -5159,7 +5147,7 @@
       </c>
       <c r="R8">
         <f>'2025 - Spring'!K7</f>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -5187,7 +5175,7 @@
       </c>
       <c r="R9">
         <f>'2025 - Spring'!K8</f>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -5215,7 +5203,7 @@
       </c>
       <c r="R10">
         <f>'2025 - Spring'!K9</f>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -5236,7 +5224,7 @@
       </c>
       <c r="R11">
         <f>'2025 - Spring'!K10</f>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -5257,7 +5245,7 @@
       </c>
       <c r="R12">
         <f>'2025 - Spring'!K11</f>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -5278,7 +5266,7 @@
       </c>
       <c r="R13">
         <f>'2025 - Spring'!K12</f>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -5299,7 +5287,7 @@
       </c>
       <c r="R14">
         <f>'2025 - Spring'!K13</f>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -5563,10 +5551,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0179C6-09EB-4EF2-AC44-670A4027DE80}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5631,10 +5619,10 @@
         <v>83</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E2" t="s">
         <v>145</v>
@@ -5649,7 +5637,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I13" si="0">SUM(G2:H2)</f>
+        <f t="shared" ref="I2:I7" si="0">SUM(G2:H2)</f>
         <v>11</v>
       </c>
       <c r="K2">
@@ -5662,33 +5650,53 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>239</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="17"/>
+        <v>83</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5</v>
+      </c>
       <c r="I3" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K3">
-        <f>K2+I3</f>
-        <v>11</v>
+        <f>I3+K2</f>
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>240</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E4" t="s">
         <v>143</v>
@@ -5701,299 +5709,189 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K13" si="1">K3+I4</f>
-        <v>11</v>
+        <f t="shared" ref="K4:K7" si="1">I4+K3</f>
+        <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>241</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="F5" s="19"/>
+      <c r="C5" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>241</v>
+      </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="17"/>
+      <c r="E6" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>244</v>
+      </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>21</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>250</v>
+      </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="D8" t="s">
-        <v>251</v>
-      </c>
-      <c r="E8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="F9" s="19"/>
-      <c r="I9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>252</v>
-      </c>
-      <c r="E10" t="s">
-        <v>145</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="L10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>245</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>247</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>248</v>
-      </c>
-      <c r="I12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="17"/>
-      <c r="I13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="24" t="s">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="2">
-        <f>SUM(G2:G13)</f>
-        <v>7</v>
-      </c>
-      <c r="H14" s="2">
-        <f>SUM(H2:H13)</f>
-        <v>4</v>
-      </c>
-      <c r="I14" s="2">
-        <f>SUM(G14:H14)</f>
-        <v>11</v>
-      </c>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="24" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="2">
+        <f>SUM(G2:G7)</f>
+        <v>12</v>
+      </c>
+      <c r="H8" s="2">
+        <f>SUM(H2:H7)</f>
+        <v>9</v>
+      </c>
+      <c r="I8" s="2">
+        <f>SUM(G8:H8)</f>
+        <v>21</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="4">
-        <f>AVERAGE(G2:G13)</f>
-        <v>7</v>
-      </c>
-      <c r="H15" s="4">
-        <f>AVERAGE(H2:H13)</f>
-        <v>4</v>
-      </c>
-      <c r="I15" s="4">
-        <f>SUM(G15:H15)</f>
-        <v>11</v>
-      </c>
-      <c r="J15" s="5" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="4">
+        <f>AVERAGE(G2:G7)</f>
+        <v>6</v>
+      </c>
+      <c r="H9" s="4">
+        <f>AVERAGE(H2:H7)</f>
+        <v>4.5</v>
+      </c>
+      <c r="I9" s="4">
+        <f>SUM(G9:H9)</f>
+        <v>10.5</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
+    <row r="10" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="6">
-        <f>I15/(64+12)</f>
-        <v>0.14473684210526316</v>
-      </c>
-      <c r="J16" s="5" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="6">
+        <f>I9/(64+12)</f>
+        <v>0.13815789473684212</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="17"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="17"/>
+    </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" s="17"/>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" s="17"/>
@@ -6003,35 +5901,17 @@
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C28" s="17"/>
-    </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C30" s="17"/>
-    </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C31" s="17"/>
-    </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C32" s="17"/>
-      <c r="D32" s="18"/>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C33" s="17"/>
-      <c r="D33" s="18"/>
+      <c r="D27" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7327,7 +7207,7 @@
         <v>143</v>
       </c>
       <c r="F14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G14" s="1">
         <v>13</v>

</xml_diff>

<commit_message>
Updated attendance for Sarah Wahby presentation
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apecseminar.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4463E591-DC8B-4124-9305-F0A29AA25A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B576231C-EE89-47BB-84EB-3D90EB407466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="769" activeTab="1" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-28920" yWindow="3780" windowWidth="29040" windowHeight="15720" tabRatio="769" activeTab="1" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance Descriptives" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="250">
   <si>
     <t>Date</t>
   </si>
@@ -772,21 +772,9 @@
     <t>Jan. 29th</t>
   </si>
   <si>
-    <t>Neural Correlates of visual attention and its correlation with consumer preferences using eye-tracking and EEG</t>
-  </si>
-  <si>
-    <t>Uma Parasuram</t>
-  </si>
-  <si>
-    <t>Runcheng Xu</t>
-  </si>
-  <si>
     <t>Reflections on the Job Market</t>
   </si>
   <si>
-    <t>Ling Yao, Monique Davis, …</t>
-  </si>
-  <si>
     <t>Ryan McWay</t>
   </si>
   <si>
@@ -806,6 +794,15 @@
   </si>
   <si>
     <t>Sarah Wahby</t>
+  </si>
+  <si>
+    <t>Ling Yao, Monique Davis,Becca Weir, Yanxu Long, Divya Pandey</t>
+  </si>
+  <si>
+    <t>May 7th</t>
+  </si>
+  <si>
+    <t>Climate change, migration and conflict in Sudan</t>
   </si>
 </sst>
 </file>
@@ -1170,13 +1167,10 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4925,28 +4919,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A92331-1E38-48FD-9605-0D81D4E71360}">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" customWidth="1"/>
-    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="11.6640625" customWidth="1"/>
-    <col min="20" max="26" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.1796875" customWidth="1"/>
+    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="11.6328125" customWidth="1"/>
+    <col min="20" max="26" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>125</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -4970,7 +4964,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>123</v>
       </c>
@@ -4998,7 +4992,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>124</v>
       </c>
@@ -5026,7 +5020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>126</v>
       </c>
@@ -5054,7 +5048,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>127</v>
       </c>
@@ -5079,10 +5073,10 @@
       </c>
       <c r="R6">
         <f>'2025 - Spring'!K5</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
       <c r="N7">
         <v>5</v>
@@ -5101,10 +5095,10 @@
       </c>
       <c r="R7">
         <f>'2025 - Spring'!K6</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>122</v>
       </c>
@@ -5127,12 +5121,8 @@
         <f>'2024 - Fall'!K7</f>
         <v>93</v>
       </c>
-      <c r="R8">
-        <f>'2025 - Spring'!K7</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>120</v>
       </c>
@@ -5156,7 +5146,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>121</v>
       </c>
@@ -5180,7 +5170,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N11">
         <v>9</v>
       </c>
@@ -5197,7 +5187,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N12">
         <v>10</v>
       </c>
@@ -5214,7 +5204,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N13">
         <v>11</v>
       </c>
@@ -5231,7 +5221,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N14">
         <v>12</v>
       </c>
@@ -5248,7 +5238,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N15">
         <v>13</v>
       </c>
@@ -5265,7 +5255,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="N16">
         <v>14</v>
       </c>
@@ -5282,7 +5272,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N17">
         <v>15</v>
       </c>
@@ -5295,17 +5285,17 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N19" s="20" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="21" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N21" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="22" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N22" t="s">
         <v>144</v>
       </c>
@@ -5316,7 +5306,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N23">
         <f>1+1+1+1+1</f>
         <v>5</v>
@@ -5330,7 +5320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N24" s="16">
         <f>N23/SUM($N$23:$P$23)</f>
         <v>0.38461538461538464</v>
@@ -5344,12 +5334,12 @@
         <v>0.23076923076923078</v>
       </c>
     </row>
-    <row r="26" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N26" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="27" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N27" t="s">
         <v>155</v>
       </c>
@@ -5390,7 +5380,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N28">
         <f>1+1+1+1+1+1+1</f>
         <v>7</v>
@@ -5444,7 +5434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="14:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="14:26" x14ac:dyDescent="0.35">
       <c r="N29" s="16">
         <f t="shared" ref="N29:Z29" si="0">N28/SUM($N$28:$Z$28)</f>
         <v>0.2413793103448276</v>
@@ -5509,29 +5499,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0179C6-09EB-4EF2-AC44-670A4027DE80}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="35.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.36328125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="35.81640625" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5569,7 +5559,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>238</v>
       </c>
@@ -5577,10 +5567,10 @@
         <v>83</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E2" t="s">
         <v>145</v>
@@ -5595,7 +5585,7 @@
         <v>4</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I7" si="0">SUM(G2:H2)</f>
+        <f t="shared" ref="I2:I5" si="0">SUM(G2:H2)</f>
         <v>11</v>
       </c>
       <c r="K2">
@@ -5606,7 +5596,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
@@ -5614,10 +5604,10 @@
         <v>83</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E3" t="s">
         <v>144</v>
@@ -5643,7 +5633,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>78</v>
       </c>
@@ -5654,7 +5644,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E4" t="s">
         <v>143</v>
@@ -5673,211 +5663,196 @@
         <v>6</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K7" si="1">I4+K3</f>
+        <f>I4+K3</f>
         <v>27</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>240</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>239</v>
+        <v>246</v>
+      </c>
+      <c r="D5" t="s">
+        <v>249</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>241</v>
+        <v>156</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f>I5+K4</f>
+        <v>32</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>81</v>
+        <v>248</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>214</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(G6:H6)</f>
         <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f>I6+K5</f>
+        <v>32</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="2">
+        <f>SUM(G2:G5)</f>
+        <v>17</v>
+      </c>
+      <c r="H7" s="2">
+        <f>SUM(H2:H5)</f>
+        <v>15</v>
+      </c>
+      <c r="I7" s="2">
+        <f>SUM(G7:H7)</f>
+        <v>32</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="24" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="2">
-        <f>SUM(G2:G7)</f>
-        <v>15</v>
-      </c>
-      <c r="H8" s="2">
-        <f>SUM(H2:H7)</f>
-        <v>12</v>
-      </c>
-      <c r="I8" s="2">
+      <c r="G8" s="4">
+        <f>AVERAGE(G2:G5)</f>
+        <v>4.25</v>
+      </c>
+      <c r="H8" s="4">
+        <f>AVERAGE(H2:H5)</f>
+        <v>3.75</v>
+      </c>
+      <c r="I8" s="4">
         <f>SUM(G8:H8)</f>
-        <v>27</v>
-      </c>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="4">
-        <f>AVERAGE(G2:G7)</f>
-        <v>5</v>
-      </c>
-      <c r="H9" s="4">
-        <f>AVERAGE(H2:H7)</f>
-        <v>4</v>
-      </c>
-      <c r="I9" s="4">
-        <f>SUM(G9:H9)</f>
-        <v>9</v>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="6">
+        <f>I8/(64+12)</f>
+        <v>0.10526315789473684</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="6">
-        <f>I9/(64+12)</f>
-        <v>0.11842105263157894</v>
-      </c>
-      <c r="J10" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="17"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="17"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="17"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="17"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="17"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="17"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="17"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" s="17"/>
       <c r="D26" s="18"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
+    <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5887,26 +5862,26 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.36328125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5944,7 +5919,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>169</v>
       </c>
@@ -5984,7 +5959,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>170</v>
       </c>
@@ -6024,7 +5999,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>171</v>
       </c>
@@ -6064,7 +6039,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>172</v>
       </c>
@@ -6104,7 +6079,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>173</v>
       </c>
@@ -6144,7 +6119,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>174</v>
       </c>
@@ -6184,7 +6159,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>175</v>
       </c>
@@ -6224,7 +6199,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>176</v>
       </c>
@@ -6264,7 +6239,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>177</v>
       </c>
@@ -6304,7 +6279,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>178</v>
       </c>
@@ -6344,7 +6319,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>179</v>
       </c>
@@ -6384,7 +6359,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>180</v>
       </c>
@@ -6424,7 +6399,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>181</v>
       </c>
@@ -6464,7 +6439,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>182</v>
       </c>
@@ -6504,7 +6479,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>183</v>
       </c>
@@ -6544,7 +6519,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
@@ -6567,7 +6542,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="24" t="s">
         <v>38</v>
       </c>
@@ -6592,7 +6567,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="24" t="s">
         <v>39</v>
       </c>
@@ -6611,43 +6586,43 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C25" s="17"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C26" s="17"/>
       <c r="D26" s="18"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C27" s="17"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C31" s="17"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C32" s="17"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C33" s="17"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C34" s="17"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C35" s="17"/>
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C36" s="17"/>
       <c r="D36" s="18"/>
     </row>
@@ -6670,21 +6645,21 @@
       <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="1" customWidth="1"/>
     <col min="3" max="3" width="26" style="8" customWidth="1"/>
-    <col min="4" max="4" width="45.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="4" max="4" width="45.81640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6719,7 +6694,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -6756,7 +6731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -6793,7 +6768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
@@ -6827,7 +6802,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>71</v>
       </c>
@@ -6864,7 +6839,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -6901,7 +6876,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -6938,7 +6913,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -6972,7 +6947,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
@@ -7009,7 +6984,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
@@ -7046,7 +7021,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>77</v>
       </c>
@@ -7083,7 +7058,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -7120,7 +7095,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>79</v>
       </c>
@@ -7154,7 +7129,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="26.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -7171,7 +7146,7 @@
         <v>143</v>
       </c>
       <c r="F14" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G14" s="1">
         <v>13</v>
@@ -7191,7 +7166,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
@@ -7228,7 +7203,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -7262,7 +7237,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
@@ -7285,7 +7260,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="24" t="s">
         <v>38</v>
       </c>
@@ -7310,7 +7285,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="24" t="s">
         <v>39</v>
       </c>
@@ -7329,29 +7304,29 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E29"/>
     </row>
   </sheetData>
@@ -7373,21 +7348,21 @@
       <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.36328125" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -7422,7 +7397,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -7459,7 +7434,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -7496,7 +7471,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -7533,7 +7508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -7567,7 +7542,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -7604,7 +7579,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -7641,7 +7616,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -7678,7 +7653,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -7715,7 +7690,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -7752,7 +7727,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -7789,7 +7764,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -7826,7 +7801,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -7860,7 +7835,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -7897,7 +7872,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -7934,7 +7909,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="24" t="s">
         <v>36</v>
       </c>
@@ -7957,7 +7932,7 @@
       </c>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="24" t="s">
         <v>38</v>
       </c>
@@ -7982,7 +7957,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="24" t="s">
         <v>39</v>
       </c>
@@ -8001,7 +7976,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A16:C16"/>
@@ -8021,12 +7996,12 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="20.77734375" customWidth="1"/>
+    <col min="1" max="8" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>117</v>
       </c>
@@ -8052,7 +8027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>118</v>
       </c>
@@ -8079,7 +8054,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
@@ -8088,7 +8063,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10"/>
@@ -8097,7 +8072,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10"/>
@@ -8106,7 +8081,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10"/>
@@ -8115,7 +8090,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="10"/>
@@ -8124,7 +8099,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10"/>
@@ -8133,7 +8108,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
@@ -8142,7 +8117,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
@@ -8151,7 +8126,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
@@ -8160,7 +8135,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="10"/>
@@ -8169,7 +8144,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="10"/>
@@ -8178,7 +8153,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="10"/>
@@ -8187,7 +8162,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="10"/>
@@ -8196,7 +8171,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="10"/>
@@ -8205,7 +8180,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="24" t="s">
         <v>36</v>
       </c>
@@ -8229,7 +8204,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="24" t="s">
         <v>38</v>
       </c>
@@ -8255,7 +8230,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="24" t="s">
         <v>39</v>
       </c>
@@ -8272,7 +8247,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A17:C17"/>

</xml_diff>

<commit_message>
Updated attendance for job market panel
</commit_message>
<xml_diff>
--- a/seminar_attendance.xlsx
+++ b/seminar_attendance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\apecseminar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B576231C-EE89-47BB-84EB-3D90EB407466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443E734A-D23E-4D82-B252-A7B947CDD517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3780" windowWidth="29040" windowHeight="15720" tabRatio="769" activeTab="1" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
+    <workbookView xWindow="-28920" yWindow="3780" windowWidth="29040" windowHeight="15720" tabRatio="769" xr2:uid="{43CE904D-F190-401C-8366-D099F1A9B15F}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance Descriptives" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="251">
   <si>
     <t>Date</t>
   </si>
@@ -803,6 +803,9 @@
   </si>
   <si>
     <t>Climate change, migration and conflict in Sudan</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1173,7 @@
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4919,8 +4922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A92331-1E38-48FD-9605-0D81D4E71360}">
   <dimension ref="A1:Z29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5095,7 +5098,7 @@
       </c>
       <c r="R7">
         <f>'2025 - Spring'!K6</f>
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -5501,8 +5504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0179C6-09EB-4EF2-AC44-670A4027DE80}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5726,13 +5729,19 @@
       <c r="F6" s="17" t="s">
         <v>240</v>
       </c>
+      <c r="G6" s="1">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>14</v>
+      </c>
       <c r="I6" s="1">
         <f>SUM(G6:H6)</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="K6">
         <f>I6+K5</f>
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>229</v>
@@ -5748,16 +5757,16 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="2">
-        <f>SUM(G2:G5)</f>
-        <v>17</v>
+        <f>SUM(G2:G6)</f>
+        <v>24</v>
       </c>
       <c r="H7" s="2">
-        <f>SUM(H2:H5)</f>
-        <v>15</v>
+        <f>SUM(H2:H6)</f>
+        <v>29</v>
       </c>
       <c r="I7" s="2">
         <f>SUM(G7:H7)</f>
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="J7" s="3"/>
     </row>
@@ -5771,16 +5780,16 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="4">
-        <f>AVERAGE(G2:G5)</f>
-        <v>4.25</v>
+        <f>AVERAGE(G2:G6)</f>
+        <v>4.8</v>
       </c>
       <c r="H8" s="4">
-        <f>AVERAGE(H2:H5)</f>
-        <v>3.75</v>
+        <f>AVERAGE(H2:H6)</f>
+        <v>5.8</v>
       </c>
       <c r="I8" s="4">
         <f>SUM(G8:H8)</f>
-        <v>8</v>
+        <v>10.6</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>40</v>
@@ -5799,13 +5808,18 @@
       <c r="H9" s="4"/>
       <c r="I9" s="6">
         <f>I8/(64+12)</f>
-        <v>0.10526315789473684</v>
+        <v>0.13947368421052631</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I13" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C15" s="17"/>
     </row>

</xml_diff>